<commit_message>
Adding first broadcasting plan ideas
</commit_message>
<xml_diff>
--- a/Sendeplan.xlsx
+++ b/Sendeplan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eris TV\git\ErisPlayer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7EAAC5F-1ACA-4F80-B9F2-741F23A4A601}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4399379C-4D71-43E9-A549-BE5F320D46A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="14">
   <si>
     <t>Montag</t>
   </si>
@@ -62,6 +62,12 @@
   </si>
   <si>
     <t>KasperKast</t>
+  </si>
+  <si>
+    <t>MS-Live?</t>
+  </si>
+  <si>
+    <t>DeutschalndNichtNormal?</t>
   </si>
 </sst>
 </file>
@@ -1761,7 +1767,7 @@
   <dimension ref="B1:R52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.453125" defaultRowHeight="18.5" x14ac:dyDescent="0.45"/>
@@ -2182,7 +2188,9 @@
       <c r="B19" s="8">
         <v>0.812500000000001</v>
       </c>
-      <c r="C19" s="19"/>
+      <c r="C19" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="D19" s="31"/>
       <c r="E19" s="20"/>
       <c r="F19" s="31"/>
@@ -2206,7 +2214,9 @@
       </c>
       <c r="C20" s="19"/>
       <c r="D20" s="31"/>
-      <c r="E20" s="20"/>
+      <c r="E20" s="20" t="s">
+        <v>13</v>
+      </c>
       <c r="F20" s="31"/>
       <c r="G20" s="20"/>
       <c r="H20" s="20"/>

</xml_diff>

<commit_message>
Sendeplan --> Adding Creators-Table
</commit_message>
<xml_diff>
--- a/Sendeplan.xlsx
+++ b/Sendeplan.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eris TV\git\ErisPlayer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4399379C-4D71-43E9-A549-BE5F320D46A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60916C09-9277-4E86-B390-44343892FA7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Default" sheetId="1" r:id="rId1"/>
-    <sheet name="Version1" sheetId="2" r:id="rId2"/>
+    <sheet name="Creator" sheetId="3" r:id="rId1"/>
+    <sheet name="Default" sheetId="1" r:id="rId2"/>
+    <sheet name="Version1" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="54">
   <si>
     <t>Montag</t>
   </si>
@@ -68,6 +69,126 @@
   </si>
   <si>
     <t>DeutschalndNichtNormal?</t>
+  </si>
+  <si>
+    <t>DVA</t>
+  </si>
+  <si>
+    <t>IDW</t>
+  </si>
+  <si>
+    <t>ClownsWelt</t>
+  </si>
+  <si>
+    <t>CLW</t>
+  </si>
+  <si>
+    <t>Dion</t>
+  </si>
+  <si>
+    <t>DIN</t>
+  </si>
+  <si>
+    <t>AOW</t>
+  </si>
+  <si>
+    <t>DerJasssen</t>
+  </si>
+  <si>
+    <t>DJA</t>
+  </si>
+  <si>
+    <t>SushiTV</t>
+  </si>
+  <si>
+    <t>STV</t>
+  </si>
+  <si>
+    <t>CLC</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Kürzel</t>
+  </si>
+  <si>
+    <t>Chanel</t>
+  </si>
+  <si>
+    <t>Format 1:</t>
+  </si>
+  <si>
+    <t>Format 2:</t>
+  </si>
+  <si>
+    <t>Format 3:</t>
+  </si>
+  <si>
+    <t>Format 4:</t>
+  </si>
+  <si>
+    <t>Format 5:</t>
+  </si>
+  <si>
+    <t>Die Vulgäre Analyse</t>
+  </si>
+  <si>
+    <t>Schlomo Finkelstin</t>
+  </si>
+  <si>
+    <t>IdiotenWatch</t>
+  </si>
+  <si>
+    <t>Kasper</t>
+  </si>
+  <si>
+    <t>Feroz Kahn</t>
+  </si>
+  <si>
+    <t>achse:ostwest</t>
+  </si>
+  <si>
+    <t>Clowny</t>
+  </si>
+  <si>
+    <t>Der Schattenmacher</t>
+  </si>
+  <si>
+    <t>Schattie</t>
+  </si>
+  <si>
+    <t>DSM</t>
+  </si>
+  <si>
+    <t>Charlotte Corday</t>
+  </si>
+  <si>
+    <t>Jassen</t>
+  </si>
+  <si>
+    <t>Sushi</t>
+  </si>
+  <si>
+    <t>KLIA</t>
+  </si>
+  <si>
+    <t>HW</t>
+  </si>
+  <si>
+    <t>Straftat der Woche</t>
+  </si>
+  <si>
+    <t>SDW</t>
+  </si>
+  <si>
+    <t>ClownsWelt3</t>
+  </si>
+  <si>
+    <t>CW3</t>
+  </si>
+  <si>
+    <t>KEK</t>
   </si>
 </sst>
 </file>
@@ -96,7 +217,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -109,8 +230,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="30">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -521,11 +654,79 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -604,13 +805,46 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -892,6 +1126,444 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDC80B26-76B8-492B-B869-87A4BA59C239}">
+  <dimension ref="B1:M44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.90625" style="36"/>
+    <col min="2" max="2" width="17.453125" style="36" customWidth="1"/>
+    <col min="3" max="14" width="23.26953125" style="36" customWidth="1"/>
+    <col min="15" max="16384" width="10.90625" style="36"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:13" ht="19" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:13" ht="19" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="J2" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" s="38" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B3" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="41" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3" s="41" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="J3" s="41" t="s">
+        <v>44</v>
+      </c>
+      <c r="K3" s="41"/>
+      <c r="L3" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="M3" s="39" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" s="42" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="42" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="J4" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" s="42"/>
+      <c r="L4" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="M4" s="43" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" ht="19" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="40"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="40"/>
+      <c r="J5" s="40"/>
+      <c r="K5" s="40"/>
+      <c r="L5" s="40"/>
+      <c r="M5" s="38"/>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B6" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" s="41"/>
+      <c r="G6" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="41"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="41"/>
+      <c r="K6" s="41"/>
+      <c r="L6" s="41"/>
+      <c r="M6" s="39"/>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B7" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="41"/>
+      <c r="D7" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="41" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" s="41"/>
+      <c r="G7" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="H7" s="41"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="41"/>
+      <c r="K7" s="41"/>
+      <c r="L7" s="41"/>
+      <c r="M7" s="39"/>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B8" s="41"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="41"/>
+      <c r="K8" s="41"/>
+      <c r="L8" s="41"/>
+      <c r="M8" s="39"/>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B9" s="41" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="41"/>
+      <c r="K9" s="41"/>
+      <c r="L9" s="41"/>
+      <c r="M9" s="39"/>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B10" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="41"/>
+      <c r="K10" s="41"/>
+      <c r="L10" s="41"/>
+      <c r="M10" s="39"/>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B11" s="41"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="41"/>
+      <c r="J11" s="41"/>
+      <c r="K11" s="41"/>
+      <c r="L11" s="41"/>
+      <c r="M11" s="39"/>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B12" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="41"/>
+      <c r="D12" s="41"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="41"/>
+      <c r="I12" s="41"/>
+      <c r="J12" s="41"/>
+      <c r="K12" s="41"/>
+      <c r="L12" s="41"/>
+      <c r="M12" s="39"/>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B13" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="41"/>
+      <c r="D13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="41"/>
+      <c r="J13" s="41"/>
+      <c r="K13" s="41"/>
+      <c r="L13" s="41"/>
+      <c r="M13" s="39"/>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B14" s="41"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="41"/>
+      <c r="I14" s="41"/>
+      <c r="J14" s="41"/>
+      <c r="K14" s="41"/>
+      <c r="L14" s="41"/>
+      <c r="M14" s="39"/>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B15" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="41"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="41"/>
+      <c r="I15" s="41"/>
+      <c r="J15" s="41"/>
+      <c r="K15" s="41"/>
+      <c r="L15" s="41"/>
+      <c r="M15" s="39"/>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B16" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="41"/>
+      <c r="I16" s="41"/>
+      <c r="J16" s="41"/>
+      <c r="K16" s="41"/>
+      <c r="L16" s="41"/>
+      <c r="M16" s="39"/>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B17" s="41"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="41"/>
+      <c r="J17" s="41"/>
+      <c r="K17" s="41"/>
+      <c r="L17" s="41"/>
+      <c r="M17" s="39"/>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B18" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="41"/>
+      <c r="J18" s="41"/>
+      <c r="K18" s="41"/>
+      <c r="L18" s="41"/>
+      <c r="M18" s="39"/>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B19" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="41"/>
+      <c r="I19" s="41"/>
+      <c r="J19" s="41"/>
+      <c r="K19" s="41"/>
+      <c r="L19" s="41"/>
+      <c r="M19" s="39"/>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B31" s="37"/>
+      <c r="C31" s="37"/>
+      <c r="D31" s="37"/>
+      <c r="E31" s="37"/>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B33" s="37"/>
+      <c r="C33" s="37"/>
+      <c r="D33" s="37"/>
+      <c r="E33" s="37"/>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="D34" s="37"/>
+      <c r="E34" s="37"/>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B35" s="37"/>
+      <c r="D35" s="37"/>
+      <c r="E35" s="37"/>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="D36" s="37"/>
+      <c r="E36" s="37"/>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="D37" s="37"/>
+      <c r="E37" s="37"/>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="D38" s="37"/>
+      <c r="E38" s="37"/>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="D39" s="37"/>
+      <c r="E39" s="37"/>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="D40" s="37"/>
+      <c r="E40" s="37"/>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="D41" s="37"/>
+      <c r="E41" s="37"/>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B42" s="37"/>
+      <c r="C42" s="37"/>
+      <c r="D42" s="37"/>
+      <c r="E42" s="37"/>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B43" s="37"/>
+      <c r="C43" s="37"/>
+      <c r="D43" s="37"/>
+      <c r="E43" s="37"/>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B44" s="37"/>
+      <c r="C44" s="37"/>
+      <c r="D44" s="37"/>
+      <c r="E44" s="37"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:R52"/>
   <sheetViews>
@@ -1762,12 +2434,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE945620-3AB5-4535-BD1C-DE4CAECAC6E0}">
   <dimension ref="B1:R52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.453125" defaultRowHeight="18.5" x14ac:dyDescent="0.45"/>
@@ -2072,7 +2744,9 @@
       <c r="B14" s="8">
         <v>0.70833333333333404</v>
       </c>
-      <c r="C14" s="19"/>
+      <c r="C14" s="19" t="s">
+        <v>20</v>
+      </c>
       <c r="D14" s="20"/>
       <c r="E14" s="20"/>
       <c r="F14" s="20"/>
@@ -2095,11 +2769,11 @@
         <v>0.72916666666666696</v>
       </c>
       <c r="C15" s="22"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
       <c r="I15" s="24"/>
       <c r="K15" s="9">
         <v>0.22916666666666599</v>
@@ -2145,7 +2819,7 @@
         <v>10</v>
       </c>
       <c r="E17" s="20"/>
-      <c r="F17" s="30" t="s">
+      <c r="F17" s="33" t="s">
         <v>11</v>
       </c>
       <c r="G17" s="20"/>
@@ -2169,7 +2843,7 @@
       <c r="C18" s="19"/>
       <c r="D18" s="31"/>
       <c r="E18" s="20"/>
-      <c r="F18" s="31"/>
+      <c r="F18" s="34"/>
       <c r="G18" s="20"/>
       <c r="H18" s="20"/>
       <c r="I18" s="28"/>
@@ -2193,7 +2867,7 @@
       </c>
       <c r="D19" s="31"/>
       <c r="E19" s="20"/>
-      <c r="F19" s="31"/>
+      <c r="F19" s="34"/>
       <c r="G19" s="20"/>
       <c r="H19" s="20"/>
       <c r="I19" s="28"/>
@@ -2217,7 +2891,7 @@
       <c r="E20" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="F20" s="31"/>
+      <c r="F20" s="34"/>
       <c r="G20" s="20"/>
       <c r="H20" s="20"/>
       <c r="I20" s="28"/>
@@ -2239,7 +2913,7 @@
       <c r="C21" s="19"/>
       <c r="D21" s="31"/>
       <c r="E21" s="20"/>
-      <c r="F21" s="31"/>
+      <c r="F21" s="34"/>
       <c r="G21" s="20"/>
       <c r="H21" s="20"/>
       <c r="I21" s="28"/>
@@ -2261,7 +2935,7 @@
       <c r="C22" s="19"/>
       <c r="D22" s="31"/>
       <c r="E22" s="20"/>
-      <c r="F22" s="31"/>
+      <c r="F22" s="34"/>
       <c r="G22" s="20"/>
       <c r="H22" s="20"/>
       <c r="I22" s="28"/>
@@ -2283,7 +2957,7 @@
       <c r="C23" s="19"/>
       <c r="D23" s="31"/>
       <c r="E23" s="20"/>
-      <c r="F23" s="31"/>
+      <c r="F23" s="34"/>
       <c r="G23" s="20"/>
       <c r="H23" s="20"/>
       <c r="I23" s="28"/>
@@ -2305,7 +2979,7 @@
       <c r="C24" s="19"/>
       <c r="D24" s="31"/>
       <c r="E24" s="20"/>
-      <c r="F24" s="31"/>
+      <c r="F24" s="34"/>
       <c r="G24" s="20"/>
       <c r="H24" s="20"/>
       <c r="I24" s="28"/>
@@ -2327,7 +3001,7 @@
       <c r="C25" s="19"/>
       <c r="D25" s="31"/>
       <c r="E25" s="20"/>
-      <c r="F25" s="31"/>
+      <c r="F25" s="34"/>
       <c r="G25" s="20"/>
       <c r="H25" s="20"/>
       <c r="I25" s="28"/>
@@ -2349,7 +3023,7 @@
       <c r="C26" s="19"/>
       <c r="D26" s="31"/>
       <c r="E26" s="20"/>
-      <c r="F26" s="31"/>
+      <c r="F26" s="34"/>
       <c r="G26" s="20"/>
       <c r="H26" s="20"/>
       <c r="I26" s="28"/>
@@ -2371,7 +3045,7 @@
       <c r="C27" s="22"/>
       <c r="D27" s="32"/>
       <c r="E27" s="23"/>
-      <c r="F27" s="32"/>
+      <c r="F27" s="35"/>
       <c r="G27" s="23"/>
       <c r="H27" s="23"/>
       <c r="I27" s="29"/>
@@ -2407,140 +3081,84 @@
       <c r="I29" s="2"/>
     </row>
     <row r="30" spans="2:18" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
     </row>
     <row r="31" spans="2:18" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
     </row>
     <row r="32" spans="2:18" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
     </row>
     <row r="33" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
     </row>
     <row r="34" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
     </row>
     <row r="35" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
     </row>
     <row r="36" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
     </row>
     <row r="37" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
     </row>
     <row r="38" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
     </row>
     <row r="39" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
     </row>
     <row r="40" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
     </row>
     <row r="41" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
     </row>
     <row r="42" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
     </row>
     <row r="43" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>

</xml_diff>

<commit_message>
ErisScheduler adding getRandom (untested)
</commit_message>
<xml_diff>
--- a/Sendeplan.xlsx
+++ b/Sendeplan.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eris TV\git\Eris-Player\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7A90252-92F6-4579-AAAB-D55034DA566C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA16325-9004-415B-BEFF-994E28CCFF5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Creator" sheetId="3" r:id="rId1"/>
-    <sheet name="Default" sheetId="1" r:id="rId2"/>
-    <sheet name="Version1" sheetId="2" r:id="rId3"/>
+    <sheet name="CSV-Export" sheetId="4" r:id="rId1"/>
+    <sheet name="Creator" sheetId="3" r:id="rId2"/>
+    <sheet name="Default" sheetId="1" r:id="rId3"/>
+    <sheet name="Version1" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="55">
   <si>
     <t>Montag</t>
   </si>
@@ -1125,10 +1126,475 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2C55154-39CE-4043-8601-6109B9EED5FE}">
+  <dimension ref="A1:G49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K34" sqref="K34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="24"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="17"/>
+    </row>
+    <row r="2" spans="1:7" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="25"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="20"/>
+    </row>
+    <row r="3" spans="1:7" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="25"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="20"/>
+    </row>
+    <row r="4" spans="1:7" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="25"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="20"/>
+    </row>
+    <row r="5" spans="1:7" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="25"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="20"/>
+    </row>
+    <row r="6" spans="1:7" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="25"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="20"/>
+    </row>
+    <row r="7" spans="1:7" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="25"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="20"/>
+    </row>
+    <row r="8" spans="1:7" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="25"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="20"/>
+    </row>
+    <row r="9" spans="1:7" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="25"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="20"/>
+    </row>
+    <row r="10" spans="1:7" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="25"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="20"/>
+    </row>
+    <row r="11" spans="1:7" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="25"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="20"/>
+    </row>
+    <row r="12" spans="1:7" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="26"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="23"/>
+    </row>
+    <row r="13" spans="1:7" ht="19" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="24"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="17"/>
+    </row>
+    <row r="14" spans="1:7" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="25"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="20"/>
+    </row>
+    <row r="15" spans="1:7" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="25"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="20"/>
+    </row>
+    <row r="16" spans="1:7" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="25"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="20"/>
+    </row>
+    <row r="17" spans="1:7" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="25"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="20"/>
+    </row>
+    <row r="18" spans="1:7" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="25"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="20"/>
+    </row>
+    <row r="19" spans="1:7" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="25"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="20"/>
+    </row>
+    <row r="20" spans="1:7" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="25"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="20"/>
+    </row>
+    <row r="21" spans="1:7" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="25"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="20"/>
+    </row>
+    <row r="22" spans="1:7" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A22" s="25"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="20"/>
+    </row>
+    <row r="23" spans="1:7" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A23" s="25"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="20"/>
+    </row>
+    <row r="24" spans="1:7" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="26"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="23"/>
+    </row>
+    <row r="25" spans="1:7" ht="19" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="15"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="17"/>
+    </row>
+    <row r="26" spans="1:7" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A26" s="18"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="20"/>
+    </row>
+    <row r="27" spans="1:7" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A27" s="18"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="20"/>
+    </row>
+    <row r="28" spans="1:7" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A28" s="18"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="20"/>
+    </row>
+    <row r="29" spans="1:7" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A29" s="18"/>
+      <c r="B29" s="19"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="20"/>
+    </row>
+    <row r="30" spans="1:7" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A30" s="18"/>
+      <c r="B30" s="19"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="20"/>
+    </row>
+    <row r="31" spans="1:7" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A31" s="18"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="20"/>
+    </row>
+    <row r="32" spans="1:7" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A32" s="18"/>
+      <c r="B32" s="19"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="20"/>
+    </row>
+    <row r="33" spans="1:7" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A33" s="18"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="20"/>
+    </row>
+    <row r="34" spans="1:7" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A34" s="18"/>
+      <c r="B34" s="19"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="20"/>
+    </row>
+    <row r="35" spans="1:7" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A35" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B35" s="19"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="20"/>
+    </row>
+    <row r="36" spans="1:7" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="21"/>
+      <c r="B36" s="21"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="23"/>
+    </row>
+    <row r="37" spans="1:7" ht="19" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="15"/>
+      <c r="B37" s="16"/>
+      <c r="C37" s="16"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="16"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="34" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A38" s="18"/>
+      <c r="B38" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="C38" s="19"/>
+      <c r="D38" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" s="19"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="34"/>
+    </row>
+    <row r="39" spans="1:7" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A39" s="18"/>
+      <c r="B39" s="37"/>
+      <c r="C39" s="19"/>
+      <c r="D39" s="40"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="34"/>
+    </row>
+    <row r="40" spans="1:7" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A40" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B40" s="37"/>
+      <c r="C40" s="19"/>
+      <c r="D40" s="40"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="19"/>
+      <c r="G40" s="34"/>
+    </row>
+    <row r="41" spans="1:7" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A41" s="18"/>
+      <c r="B41" s="37"/>
+      <c r="C41" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D41" s="40"/>
+      <c r="E41" s="19"/>
+      <c r="F41" s="19"/>
+      <c r="G41" s="34"/>
+    </row>
+    <row r="42" spans="1:7" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A42" s="18"/>
+      <c r="B42" s="37"/>
+      <c r="C42" s="19"/>
+      <c r="D42" s="40"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19"/>
+      <c r="G42" s="34"/>
+    </row>
+    <row r="43" spans="1:7" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A43" s="18"/>
+      <c r="B43" s="37"/>
+      <c r="C43" s="19"/>
+      <c r="D43" s="40"/>
+      <c r="E43" s="19"/>
+      <c r="F43" s="19"/>
+      <c r="G43" s="34"/>
+    </row>
+    <row r="44" spans="1:7" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A44" s="18"/>
+      <c r="B44" s="37"/>
+      <c r="C44" s="19"/>
+      <c r="D44" s="40"/>
+      <c r="E44" s="19"/>
+      <c r="F44" s="19"/>
+      <c r="G44" s="34"/>
+    </row>
+    <row r="45" spans="1:7" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A45" s="18"/>
+      <c r="B45" s="37"/>
+      <c r="C45" s="19"/>
+      <c r="D45" s="40"/>
+      <c r="E45" s="19"/>
+      <c r="F45" s="19"/>
+      <c r="G45" s="34"/>
+    </row>
+    <row r="46" spans="1:7" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A46" s="18"/>
+      <c r="B46" s="37"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="40"/>
+      <c r="E46" s="19"/>
+      <c r="F46" s="19"/>
+      <c r="G46" s="34"/>
+    </row>
+    <row r="47" spans="1:7" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A47" s="18"/>
+      <c r="B47" s="37"/>
+      <c r="C47" s="19"/>
+      <c r="D47" s="40"/>
+      <c r="E47" s="19"/>
+      <c r="F47" s="19"/>
+      <c r="G47" s="34"/>
+    </row>
+    <row r="48" spans="1:7" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A48" s="21"/>
+      <c r="B48" s="38"/>
+      <c r="C48" s="22"/>
+      <c r="D48" s="41"/>
+      <c r="E48" s="22"/>
+      <c r="F48" s="22"/>
+      <c r="G48" s="35"/>
+    </row>
+    <row r="49" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="G37:G48"/>
+    <mergeCell ref="B38:B48"/>
+    <mergeCell ref="D38:D48"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDC80B26-76B8-492B-B869-87A4BA59C239}">
   <dimension ref="B1:M19"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -1497,7 +1963,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:R28"/>
   <sheetViews>
@@ -2121,12 +2587,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE945620-3AB5-4535-BD1C-DE4CAECAC6E0}">
-  <dimension ref="B1:R52"/>
+  <dimension ref="B1:R80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32:I79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.453125" defaultRowHeight="18.5" x14ac:dyDescent="0.45"/>
@@ -2753,29 +3219,456 @@
     <row r="29" spans="2:18" ht="21" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="30" spans="2:18" ht="21" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="31" spans="2:18" ht="21" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="32" spans="2:18" ht="21" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="33" ht="21" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="34" ht="21" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="35" ht="21" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="36" ht="21" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="37" ht="21" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="38" ht="21" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="39" ht="21" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="40" ht="21" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="41" ht="21" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="42" ht="21" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="43" ht="21" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="44" ht="21" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="45" ht="21" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="46" ht="21" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="47" ht="21" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="48" ht="21" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="49" ht="21" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="50" ht="21" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="51" ht="21" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="52" ht="21" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="32" spans="2:18" ht="21" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C32" s="24"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="16"/>
+      <c r="H32" s="16"/>
+      <c r="I32" s="17"/>
+    </row>
+    <row r="33" spans="3:9" ht="21" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C33" s="25"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="19"/>
+      <c r="H33" s="19"/>
+      <c r="I33" s="20"/>
+    </row>
+    <row r="34" spans="3:9" ht="21" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C34" s="25"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="19"/>
+      <c r="H34" s="19"/>
+      <c r="I34" s="20"/>
+    </row>
+    <row r="35" spans="3:9" ht="21" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C35" s="25"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="19"/>
+      <c r="H35" s="19"/>
+      <c r="I35" s="20"/>
+    </row>
+    <row r="36" spans="3:9" ht="21" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C36" s="25"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="19"/>
+      <c r="H36" s="19"/>
+      <c r="I36" s="20"/>
+    </row>
+    <row r="37" spans="3:9" ht="21" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C37" s="25"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="19"/>
+      <c r="H37" s="19"/>
+      <c r="I37" s="20"/>
+    </row>
+    <row r="38" spans="3:9" ht="21" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C38" s="25"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="19"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="19"/>
+      <c r="H38" s="19"/>
+      <c r="I38" s="20"/>
+    </row>
+    <row r="39" spans="3:9" ht="21" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C39" s="25"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="19"/>
+      <c r="H39" s="19"/>
+      <c r="I39" s="20"/>
+    </row>
+    <row r="40" spans="3:9" ht="21" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C40" s="25"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="19"/>
+      <c r="G40" s="19"/>
+      <c r="H40" s="19"/>
+      <c r="I40" s="20"/>
+    </row>
+    <row r="41" spans="3:9" ht="21" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C41" s="25"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="19"/>
+      <c r="F41" s="19"/>
+      <c r="G41" s="19"/>
+      <c r="H41" s="19"/>
+      <c r="I41" s="20"/>
+    </row>
+    <row r="42" spans="3:9" ht="21" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C42" s="25"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19"/>
+      <c r="G42" s="19"/>
+      <c r="H42" s="19"/>
+      <c r="I42" s="20"/>
+    </row>
+    <row r="43" spans="3:9" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C43" s="26"/>
+      <c r="D43" s="22"/>
+      <c r="E43" s="22"/>
+      <c r="F43" s="22"/>
+      <c r="G43" s="22"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="23"/>
+    </row>
+    <row r="44" spans="3:9" ht="21" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="C44" s="24"/>
+      <c r="D44" s="16"/>
+      <c r="E44" s="16"/>
+      <c r="F44" s="16"/>
+      <c r="G44" s="16"/>
+      <c r="H44" s="16"/>
+      <c r="I44" s="17"/>
+    </row>
+    <row r="45" spans="3:9" ht="21" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C45" s="25"/>
+      <c r="D45" s="19"/>
+      <c r="E45" s="19"/>
+      <c r="F45" s="19"/>
+      <c r="G45" s="19"/>
+      <c r="H45" s="19"/>
+      <c r="I45" s="20"/>
+    </row>
+    <row r="46" spans="3:9" ht="21" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C46" s="25"/>
+      <c r="D46" s="19"/>
+      <c r="E46" s="19"/>
+      <c r="F46" s="19"/>
+      <c r="G46" s="19"/>
+      <c r="H46" s="19"/>
+      <c r="I46" s="20"/>
+    </row>
+    <row r="47" spans="3:9" ht="21" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C47" s="25"/>
+      <c r="D47" s="19"/>
+      <c r="E47" s="19"/>
+      <c r="F47" s="19"/>
+      <c r="G47" s="19"/>
+      <c r="H47" s="19"/>
+      <c r="I47" s="20"/>
+    </row>
+    <row r="48" spans="3:9" ht="21" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C48" s="25"/>
+      <c r="D48" s="19"/>
+      <c r="E48" s="19"/>
+      <c r="F48" s="19"/>
+      <c r="G48" s="19"/>
+      <c r="H48" s="19"/>
+      <c r="I48" s="20"/>
+    </row>
+    <row r="49" spans="3:9" ht="21" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C49" s="25"/>
+      <c r="D49" s="19"/>
+      <c r="E49" s="19"/>
+      <c r="F49" s="19"/>
+      <c r="G49" s="19"/>
+      <c r="H49" s="19"/>
+      <c r="I49" s="20"/>
+    </row>
+    <row r="50" spans="3:9" ht="21" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C50" s="25"/>
+      <c r="D50" s="19"/>
+      <c r="E50" s="19"/>
+      <c r="F50" s="19"/>
+      <c r="G50" s="19"/>
+      <c r="H50" s="19"/>
+      <c r="I50" s="20"/>
+    </row>
+    <row r="51" spans="3:9" ht="21" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C51" s="25"/>
+      <c r="D51" s="19"/>
+      <c r="E51" s="19"/>
+      <c r="F51" s="19"/>
+      <c r="G51" s="19"/>
+      <c r="H51" s="19"/>
+      <c r="I51" s="20"/>
+    </row>
+    <row r="52" spans="3:9" ht="21" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C52" s="25"/>
+      <c r="D52" s="19"/>
+      <c r="E52" s="19"/>
+      <c r="F52" s="19"/>
+      <c r="G52" s="19"/>
+      <c r="H52" s="19"/>
+      <c r="I52" s="20"/>
+    </row>
+    <row r="53" spans="3:9" x14ac:dyDescent="0.45">
+      <c r="C53" s="25"/>
+      <c r="D53" s="19"/>
+      <c r="E53" s="19"/>
+      <c r="F53" s="19"/>
+      <c r="G53" s="19"/>
+      <c r="H53" s="19"/>
+      <c r="I53" s="20"/>
+    </row>
+    <row r="54" spans="3:9" x14ac:dyDescent="0.45">
+      <c r="C54" s="25"/>
+      <c r="D54" s="19"/>
+      <c r="E54" s="19"/>
+      <c r="F54" s="19"/>
+      <c r="G54" s="19"/>
+      <c r="H54" s="19"/>
+      <c r="I54" s="20"/>
+    </row>
+    <row r="55" spans="3:9" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C55" s="26"/>
+      <c r="D55" s="22"/>
+      <c r="E55" s="22"/>
+      <c r="F55" s="22"/>
+      <c r="G55" s="22"/>
+      <c r="H55" s="22"/>
+      <c r="I55" s="23"/>
+    </row>
+    <row r="56" spans="3:9" ht="19" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="C56" s="15"/>
+      <c r="D56" s="16"/>
+      <c r="E56" s="16"/>
+      <c r="F56" s="16"/>
+      <c r="G56" s="16"/>
+      <c r="H56" s="16"/>
+      <c r="I56" s="17"/>
+    </row>
+    <row r="57" spans="3:9" x14ac:dyDescent="0.45">
+      <c r="C57" s="18"/>
+      <c r="D57" s="19"/>
+      <c r="E57" s="19"/>
+      <c r="F57" s="19"/>
+      <c r="G57" s="19"/>
+      <c r="H57" s="19"/>
+      <c r="I57" s="20"/>
+    </row>
+    <row r="58" spans="3:9" x14ac:dyDescent="0.45">
+      <c r="C58" s="18"/>
+      <c r="D58" s="19"/>
+      <c r="E58" s="19"/>
+      <c r="F58" s="19"/>
+      <c r="G58" s="19"/>
+      <c r="H58" s="19"/>
+      <c r="I58" s="20"/>
+    </row>
+    <row r="59" spans="3:9" x14ac:dyDescent="0.45">
+      <c r="C59" s="18"/>
+      <c r="D59" s="19"/>
+      <c r="E59" s="19"/>
+      <c r="F59" s="19"/>
+      <c r="G59" s="19"/>
+      <c r="H59" s="19"/>
+      <c r="I59" s="20"/>
+    </row>
+    <row r="60" spans="3:9" x14ac:dyDescent="0.45">
+      <c r="C60" s="18"/>
+      <c r="D60" s="19"/>
+      <c r="E60" s="19"/>
+      <c r="F60" s="19"/>
+      <c r="G60" s="19"/>
+      <c r="H60" s="19"/>
+      <c r="I60" s="20"/>
+    </row>
+    <row r="61" spans="3:9" x14ac:dyDescent="0.45">
+      <c r="C61" s="18"/>
+      <c r="D61" s="19"/>
+      <c r="E61" s="19"/>
+      <c r="F61" s="19"/>
+      <c r="G61" s="19"/>
+      <c r="H61" s="19"/>
+      <c r="I61" s="20"/>
+    </row>
+    <row r="62" spans="3:9" x14ac:dyDescent="0.45">
+      <c r="C62" s="18"/>
+      <c r="D62" s="19"/>
+      <c r="E62" s="19"/>
+      <c r="F62" s="19"/>
+      <c r="G62" s="19"/>
+      <c r="H62" s="19"/>
+      <c r="I62" s="20"/>
+    </row>
+    <row r="63" spans="3:9" x14ac:dyDescent="0.45">
+      <c r="C63" s="18"/>
+      <c r="D63" s="19"/>
+      <c r="E63" s="19"/>
+      <c r="F63" s="19"/>
+      <c r="G63" s="19"/>
+      <c r="H63" s="19"/>
+      <c r="I63" s="20"/>
+    </row>
+    <row r="64" spans="3:9" x14ac:dyDescent="0.45">
+      <c r="C64" s="18"/>
+      <c r="D64" s="19"/>
+      <c r="E64" s="19"/>
+      <c r="F64" s="19"/>
+      <c r="G64" s="19"/>
+      <c r="H64" s="19"/>
+      <c r="I64" s="20"/>
+    </row>
+    <row r="65" spans="3:9" x14ac:dyDescent="0.45">
+      <c r="C65" s="18"/>
+      <c r="D65" s="19"/>
+      <c r="E65" s="19"/>
+      <c r="F65" s="19"/>
+      <c r="G65" s="19"/>
+      <c r="H65" s="19"/>
+      <c r="I65" s="20"/>
+    </row>
+    <row r="66" spans="3:9" x14ac:dyDescent="0.45">
+      <c r="C66" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="D66" s="19"/>
+      <c r="E66" s="19"/>
+      <c r="F66" s="19"/>
+      <c r="G66" s="19"/>
+      <c r="H66" s="19"/>
+      <c r="I66" s="20"/>
+    </row>
+    <row r="67" spans="3:9" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C67" s="21"/>
+      <c r="D67" s="21"/>
+      <c r="E67" s="21"/>
+      <c r="F67" s="21"/>
+      <c r="G67" s="21"/>
+      <c r="H67" s="21"/>
+      <c r="I67" s="23"/>
+    </row>
+    <row r="68" spans="3:9" ht="19" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="C68" s="15"/>
+      <c r="D68" s="16"/>
+      <c r="E68" s="16"/>
+      <c r="F68" s="16"/>
+      <c r="G68" s="16"/>
+      <c r="H68" s="16"/>
+      <c r="I68" s="34" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="69" spans="3:9" x14ac:dyDescent="0.45">
+      <c r="C69" s="18"/>
+      <c r="D69" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="E69" s="19"/>
+      <c r="F69" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="G69" s="19"/>
+      <c r="H69" s="19"/>
+      <c r="I69" s="34"/>
+    </row>
+    <row r="70" spans="3:9" x14ac:dyDescent="0.45">
+      <c r="C70" s="18"/>
+      <c r="D70" s="37"/>
+      <c r="E70" s="19"/>
+      <c r="F70" s="40"/>
+      <c r="G70" s="19"/>
+      <c r="H70" s="19"/>
+      <c r="I70" s="34"/>
+    </row>
+    <row r="71" spans="3:9" x14ac:dyDescent="0.45">
+      <c r="C71" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D71" s="37"/>
+      <c r="E71" s="19"/>
+      <c r="F71" s="40"/>
+      <c r="G71" s="19"/>
+      <c r="H71" s="19"/>
+      <c r="I71" s="34"/>
+    </row>
+    <row r="72" spans="3:9" x14ac:dyDescent="0.45">
+      <c r="C72" s="18"/>
+      <c r="D72" s="37"/>
+      <c r="E72" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="F72" s="40"/>
+      <c r="G72" s="19"/>
+      <c r="H72" s="19"/>
+      <c r="I72" s="34"/>
+    </row>
+    <row r="73" spans="3:9" x14ac:dyDescent="0.45">
+      <c r="C73" s="18"/>
+      <c r="D73" s="37"/>
+      <c r="E73" s="19"/>
+      <c r="F73" s="40"/>
+      <c r="G73" s="19"/>
+      <c r="H73" s="19"/>
+      <c r="I73" s="34"/>
+    </row>
+    <row r="74" spans="3:9" x14ac:dyDescent="0.45">
+      <c r="C74" s="18"/>
+      <c r="D74" s="37"/>
+      <c r="E74" s="19"/>
+      <c r="F74" s="40"/>
+      <c r="G74" s="19"/>
+      <c r="H74" s="19"/>
+      <c r="I74" s="34"/>
+    </row>
+    <row r="75" spans="3:9" x14ac:dyDescent="0.45">
+      <c r="C75" s="18"/>
+      <c r="D75" s="37"/>
+      <c r="E75" s="19"/>
+      <c r="F75" s="40"/>
+      <c r="G75" s="19"/>
+      <c r="H75" s="19"/>
+      <c r="I75" s="34"/>
+    </row>
+    <row r="76" spans="3:9" x14ac:dyDescent="0.45">
+      <c r="C76" s="18"/>
+      <c r="D76" s="37"/>
+      <c r="E76" s="19"/>
+      <c r="F76" s="40"/>
+      <c r="G76" s="19"/>
+      <c r="H76" s="19"/>
+      <c r="I76" s="34"/>
+    </row>
+    <row r="77" spans="3:9" x14ac:dyDescent="0.45">
+      <c r="C77" s="18"/>
+      <c r="D77" s="37"/>
+      <c r="E77" s="19"/>
+      <c r="F77" s="40"/>
+      <c r="G77" s="19"/>
+      <c r="H77" s="19"/>
+      <c r="I77" s="34"/>
+    </row>
+    <row r="78" spans="3:9" x14ac:dyDescent="0.45">
+      <c r="C78" s="18"/>
+      <c r="D78" s="37"/>
+      <c r="E78" s="19"/>
+      <c r="F78" s="40"/>
+      <c r="G78" s="19"/>
+      <c r="H78" s="19"/>
+      <c r="I78" s="34"/>
+    </row>
+    <row r="79" spans="3:9" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C79" s="21"/>
+      <c r="D79" s="38"/>
+      <c r="E79" s="22"/>
+      <c r="F79" s="41"/>
+      <c r="G79" s="22"/>
+      <c r="H79" s="22"/>
+      <c r="I79" s="35"/>
+    </row>
+    <row r="80" spans="3:9" ht="19" thickTop="1" x14ac:dyDescent="0.45"/>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="6">
+    <mergeCell ref="I68:I79"/>
+    <mergeCell ref="D69:D79"/>
+    <mergeCell ref="F69:F79"/>
     <mergeCell ref="I16:I27"/>
     <mergeCell ref="D17:D27"/>
     <mergeCell ref="F17:F27"/>

</xml_diff>